<commit_message>
Mejoras reporte de permanencia
</commit_message>
<xml_diff>
--- a/App.Web/App_Data/GDPermanencia.xlsx
+++ b/App.Web/App_Data/GDPermanencia.xlsx
@@ -5,20 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\source\repos\GestionProcesosV2\App.Web\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsilva\source\repos\GestionProcesos\App.Web\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE0F436-893A-489E-8AFF-3250E4E25C66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37435948-6AC6-42A8-B3BA-7A391AD239C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="-120" windowWidth="23295" windowHeight="13740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="3" r:id="rId1"/>
+    <sheet name="Resumen" sheetId="3" r:id="rId1"/>
+    <sheet name="Detalle" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Detalle!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Resumen!$A$1:$E$1</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Unidad</t>
   </si>
@@ -43,6 +45,18 @@
   </si>
   <si>
     <t>Código unidad</t>
+  </si>
+  <si>
+    <t>Proceso Id</t>
+  </si>
+  <si>
+    <t>Cantidad de veces que el documento ingresa a la unidad</t>
+  </si>
+  <si>
+    <t>Total tiempo de permanencia</t>
+  </si>
+  <si>
+    <t>Unidad origen</t>
   </si>
 </sst>
 </file>
@@ -369,7 +383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F18CA003-2129-4ECA-8F4B-D4AAE8FBC4CD}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -404,4 +418,41 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995FA1DD-3E7C-4701-81BE-0A85DB2CE947}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="54.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E1" xr:uid="{211F4496-0AAC-4EB6-9DAA-87BDF49FEB35}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Reporte de permanencia de documentos
</commit_message>
<xml_diff>
--- a/App.Web/App_Data/GDPermanencia.xlsx
+++ b/App.Web/App_Data/GDPermanencia.xlsx
@@ -5,20 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsilva\source\repos\GestionProcesos\App.Web\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\source\repos\GestionProcesosV2\App.Web\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37435948-6AC6-42A8-B3BA-7A391AD239C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C30FF5E-4CE9-4C60-8B1C-DF416DB01910}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="23310" windowHeight="13740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Resumen" sheetId="3" r:id="rId1"/>
-    <sheet name="Detalle" sheetId="4" r:id="rId2"/>
+    <sheet name="Detalle" sheetId="4" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Detalle!$A$1:$E$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Resumen!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Detalle!$A$6:$D$6</definedName>
   </definedNames>
   <calcPr calcId="0"/>
   <extLst>
@@ -32,38 +30,38 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>Unidad</t>
-  </si>
-  <si>
-    <t>Promedio ingresos diarios</t>
-  </si>
-  <si>
-    <t>Promedio días de tramitación</t>
-  </si>
-  <si>
-    <t>Número de documentos creados</t>
-  </si>
-  <si>
-    <t>Código unidad</t>
-  </si>
-  <si>
     <t>Proceso Id</t>
   </si>
   <si>
-    <t>Cantidad de veces que el documento ingresa a la unidad</t>
-  </si>
-  <si>
-    <t>Total tiempo de permanencia</t>
-  </si>
-  <si>
     <t>Unidad origen</t>
+  </si>
+  <si>
+    <t>Reporte permanencia documentos</t>
+  </si>
+  <si>
+    <t>Desde</t>
+  </si>
+  <si>
+    <t>Hasta:</t>
+  </si>
+  <si>
+    <t>Para el cálculo de fechas, se consideran solo días laborales entre 9 y 18 horas. Se excluyen días sábado, domingo y festivos.</t>
+  </si>
+  <si>
+    <t>Total tiempo de permanencia (días)</t>
+  </si>
+  <si>
+    <t>Unidad de permanencia:</t>
+  </si>
+  <si>
+    <t>Cantidad de veces que el documento ingresó a la unidad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -73,6 +71,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -98,9 +103,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,79 +390,63 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F18CA003-2129-4ECA-8F4B-D4AAE8FBC4CD}">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="57.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.28515625" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{7934493C-439C-4BC7-81C8-5D1A4AC1442F}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995FA1DD-3E7C-4701-81BE-0A85DB2CE947}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="1" max="1" width="44.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="54.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4"/>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{211F4496-0AAC-4EB6-9DAA-87BDF49FEB35}"/>
+  <autoFilter ref="A6:D6" xr:uid="{211F4496-0AAC-4EB6-9DAA-87BDF49FEB35}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mejoras filtros reporte permanencia
</commit_message>
<xml_diff>
--- a/App.Web/App_Data/GDPermanencia.xlsx
+++ b/App.Web/App_Data/GDPermanencia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\source\repos\GestionProcesosV2\App.Web\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C30FF5E-4CE9-4C60-8B1C-DF416DB01910}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA49310-86D3-4A02-ABEE-C127B7014D52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="23310" windowHeight="13740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Detalle" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Proceso Id</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Hasta:</t>
   </si>
   <si>
-    <t>Para el cálculo de fechas, se consideran solo días laborales entre 9 y 18 horas. Se excluyen días sábado, domingo y festivos.</t>
-  </si>
-  <si>
     <t>Total tiempo de permanencia (días)</t>
   </si>
   <si>
@@ -55,6 +52,18 @@
   </si>
   <si>
     <t>Cantidad de veces que el documento ingresó a la unidad</t>
+  </si>
+  <si>
+    <t>Condiciones:</t>
+  </si>
+  <si>
+    <t>Para los filtros y cálculos se utiliza la fecha de envío de las tareas. Solo se consideran días laborales entre 9 y 18 horas.</t>
+  </si>
+  <si>
+    <t>Se consideran procesos de gestión documental generados fuera de la unidad de permanencia y con estado no anulado.</t>
+  </si>
+  <si>
+    <t>Se consideran procesos que fueron atendidos por la unidad de permanencia. No se consideran procesos cerrados en la unidad de permanencia.</t>
   </si>
 </sst>
 </file>
@@ -110,7 +119,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,7 +411,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="54.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -409,13 +420,17 @@
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -423,12 +438,18 @@
         <v>3</v>
       </c>
       <c r="B3" s="4"/>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="4"/>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -438,10 +459,10 @@
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>